<commit_message>
rename everything in english
</commit_message>
<xml_diff>
--- a/Budget-Book-Template.xlsx
+++ b/Budget-Book-Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pfrom\Documents\GitHub\bank_statement_parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pfrom\Documents\GitHub\bank-account-statement-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BECBE8A-F675-4F7C-8199-6E7DE4E8798B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EF63C5-EDAF-4559-A85D-050AAF4DF652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4695" yWindow="6480" windowWidth="20685" windowHeight="12165" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>January</t>
   </si>
@@ -77,28 +77,25 @@
     <t>Average per Month</t>
   </si>
   <si>
-    <t>Kontostand</t>
-  </si>
-  <si>
-    <t>Einnahmen</t>
-  </si>
-  <si>
-    <t>Ausgaben</t>
-  </si>
-  <si>
-    <t>Bilanz</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>OBERKATEGORIE</t>
-  </si>
-  <si>
-    <t>UNTERKATEGORIE</t>
-  </si>
-  <si>
-    <t>SONSTIGES</t>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>CATEGORIES</t>
+  </si>
+  <si>
+    <t>SUBCATEGORY</t>
+  </si>
+  <si>
+    <t>TOP-CATEGORY</t>
+  </si>
+  <si>
+    <t>OTHERS</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1031,7 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,7 +1282,7 @@
     </row>
     <row r="5" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:N5" ca="1" si="2">SUM(C3:C4)</f>
@@ -1351,7 +1348,7 @@
     </row>
     <row r="7" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1435,7 +1432,7 @@
     <row r="9" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="3"/>
@@ -1497,7 +1494,7 @@
     </row>
     <row r="10" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="18">

</xml_diff>

<commit_message>
Fixed issues #16 and #15
</commit_message>
<xml_diff>
--- a/Budget-Book-Template.xlsx
+++ b/Budget-Book-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pfrom\Documents\GitHub\bank-account-statement-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8B920B-1CC0-4C33-87B7-2948A19B0C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D02BE0-B535-4113-BBC9-A3362372E9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,28 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
@@ -77,22 +99,22 @@
     <t>Average per Month</t>
   </si>
   <si>
+    <t>Kontostand</t>
+  </si>
+  <si>
+    <t>Einkommen</t>
+  </si>
+  <si>
+    <t>Ausgaben</t>
+  </si>
+  <si>
+    <t>Bilanz</t>
+  </si>
+  <si>
+    <t>Kategorien</t>
+  </si>
+  <si>
     <t>Sonstiges</t>
-  </si>
-  <si>
-    <t>Kategorien</t>
-  </si>
-  <si>
-    <t>Kontostand</t>
-  </si>
-  <si>
-    <t>Einkommen</t>
-  </si>
-  <si>
-    <t>Ausgaben</t>
-  </si>
-  <si>
-    <t>Bilanz</t>
   </si>
 </sst>
 </file>
@@ -544,7 +566,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F5F6-4B71-9470-84649FD0B0A5}"/>
+              <c16:uniqueId val="{00000000-7685-4093-A9A0-961DC285DD03}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1024,7 +1046,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1093,55 +1115,55 @@
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3">
-        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!C2:C"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))),$A2,INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A")))), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="3">
-        <f t="array" aca="1" ref="D2" ca="1">IFERROR(INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+2), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="3">
-        <f t="array" aca="1" ref="E2" ca="1">IFERROR(INDIRECT("'"&amp;E$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;E$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+2), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="3">
-        <f t="array" aca="1" ref="F2" ca="1">IFERROR(INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+2), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="3">
-        <f t="array" aca="1" ref="G2" ca="1">IFERROR(INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+2), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="3">
-        <f t="array" aca="1" ref="H2" ca="1">IFERROR(INDIRECT("'"&amp;H$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;H$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+2), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="3">
-        <f t="array" aca="1" ref="I2" ca="1">IFERROR(INDIRECT("'"&amp;I$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;I$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+2), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="array" aca="1" ref="J2" ca="1">IFERROR(INDIRECT("'"&amp;J$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;J$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+2), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="3">
-        <f t="array" aca="1" ref="K2" ca="1">IFERROR(INDIRECT("'"&amp;K$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;K$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+2), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <f t="array" aca="1" ref="L2" ca="1">IFERROR(INDIRECT("'"&amp;L$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;L$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+2), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="M2" s="3">
-        <f t="array" aca="1" ref="M2" ca="1">IFERROR(INDIRECT("'"&amp;M$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;M$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+2), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="N2" s="3">
-        <f t="array" aca="1" ref="N2" ca="1">IFERROR(INDIRECT("'"&amp;N$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;N$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+2), 0)</f>
+      <c r="C2" s="3" cm="1">
+        <f t="array" aca="1" ref="C2" ca="1">IFERROR(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" cm="1">
+        <f t="array" aca="1" ref="D2" ca="1">IFERROR(INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" cm="1">
+        <f t="array" aca="1" ref="E2" ca="1">IFERROR(INDIRECT("'"&amp;E$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;E$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" cm="1">
+        <f t="array" aca="1" ref="F2" ca="1">IFERROR(INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" cm="1">
+        <f t="array" aca="1" ref="G2" ca="1">IFERROR(INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="3" cm="1">
+        <f t="array" aca="1" ref="H2" ca="1">IFERROR(INDIRECT("'"&amp;H$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;H$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="3" cm="1">
+        <f t="array" aca="1" ref="I2" ca="1">IFERROR(INDIRECT("'"&amp;I$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;I$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="3" cm="1">
+        <f t="array" aca="1" ref="J2" ca="1">IFERROR(INDIRECT("'"&amp;J$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;J$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="3" cm="1">
+        <f t="array" aca="1" ref="K2" ca="1">IFERROR(INDIRECT("'"&amp;K$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;K$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="3" cm="1">
+        <f t="array" aca="1" ref="L2" ca="1">IFERROR(INDIRECT("'"&amp;L$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;L$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="3" cm="1">
+        <f t="array" aca="1" ref="M2" ca="1">IFERROR(INDIRECT("'"&amp;M$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;M$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="3" cm="1">
+        <f t="array" aca="1" ref="N2" ca="1">IFERROR(INDIRECT("'"&amp;N$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;N$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
         <v>0</v>
       </c>
       <c r="O2" s="3"/>
@@ -1153,14 +1175,14 @@
     </row>
     <row r="3" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3">
-        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;C1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1),"&gt;0",INDIRECT("'"&amp;C1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1)), 0)</f>
+        <f t="shared" ref="C3:E3" ca="1" si="0">IFERROR(SUMIF(INDIRECT("'"&amp;C1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1),"&gt;0",INDIRECT("'"&amp;C1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1)), 0)</f>
         <v>0</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:N3" ca="1" si="0">IFERROR(SUMIF(INDIRECT("'"&amp;D1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1),"&gt;0",INDIRECT("'"&amp;D1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1)), 0)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="E3">
@@ -1168,39 +1190,39 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;F1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1),"&gt;0",INDIRECT("'"&amp;F1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1)), 0)</f>
         <v>0</v>
       </c>
       <c r="G3">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="G3:N3" ca="1" si="1">IFERROR(SUMIF(INDIRECT("'"&amp;G1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1),"&gt;0",INDIRECT("'"&amp;G1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1)), 0)</f>
         <v>0</v>
       </c>
       <c r="H3">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="I3">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J3">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="K3">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="L3">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="M3">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="N3">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="P3" s="6">
@@ -1214,54 +1236,54 @@
     </row>
     <row r="4" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4">
-        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1),"&lt;0",INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1)), 0)</f>
+        <f t="shared" ref="C4:E4" ca="1" si="2">IFERROR(SUMIF(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1),"&lt;0",INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1)), 0)</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:N4" ca="1" si="1">IFERROR(SUMIF(INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1),"&lt;0",INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1)), 0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1),"&lt;0",INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1)), 0)</f>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ref="G4:N4" ca="1" si="3">IFERROR(SUMIF(INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1),"&lt;0",INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1)), 0)</f>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="P4" s="6">
@@ -1275,54 +1297,54 @@
     </row>
     <row r="5" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:N5" ca="1" si="2">SUM(C3:C4)</f>
+        <f t="shared" ref="C5:N5" ca="1" si="4">SUM(C3:C4)</f>
         <v>0</v>
       </c>
       <c r="D5">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="E5">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="F5">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="G5">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="H5">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="I5">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="J5">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="K5">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="L5">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="M5">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="N5">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="P5" s="6">
@@ -1341,7 +1363,7 @@
     </row>
     <row r="7" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1362,55 +1384,55 @@
     </row>
     <row r="8" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="16">
-        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;IF(ISBLANK($A8),"E2:E","C2:C")&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1),IF(ISBLANK($A8),$B$8:$B$8,$A$8:$A$8),INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1)), 0)</f>
+        <f t="shared" ref="C8:N8" ca="1" si="5">IFERROR(SUMIF(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;IF(ISBLANK($A8),"E2:E","C2:C")&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1),IF(ISBLANK($A8),$B$8:$B$8,$A$8:$A$8),INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1)), 0)</f>
         <v>0</v>
       </c>
       <c r="D8" s="16">
-        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;IF(ISBLANK($A8),"E2:E","C2:C")&amp;MAX(INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1),IF(ISBLANK($A8),$B$8:$B$8,$A$8:$A$8),INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1)), 0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="E8" s="16">
-        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;E$1&amp;" "&amp;$A$1&amp;"'!"&amp;IF(ISBLANK($A8),"E2:E","C2:C")&amp;MAX(INDIRECT("'"&amp;E$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1),IF(ISBLANK($A8),$B$8:$B$8,$A$8:$A$8),INDIRECT("'"&amp;E$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;E$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1)), 0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="F8" s="16">
-        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;IF(ISBLANK($A8),"E2:E","C2:C")&amp;MAX(INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1),IF(ISBLANK($A8),$B$8:$B$8,$A$8:$A$8),INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1)), 0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="G8" s="16">
-        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;IF(ISBLANK($A8),"E2:E","C2:C")&amp;MAX(INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1),IF(ISBLANK($A8),$B$8:$B$8,$A$8:$A$8),INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1)), 0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="H8" s="16">
-        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;H$1&amp;" "&amp;$A$1&amp;"'!"&amp;IF(ISBLANK($A8),"E2:E","C2:C")&amp;MAX(INDIRECT("'"&amp;H$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1),IF(ISBLANK($A8),$B$8:$B$8,$A$8:$A$8),INDIRECT("'"&amp;H$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;H$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1)), 0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="I8" s="16">
-        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;I$1&amp;" "&amp;$A$1&amp;"'!"&amp;IF(ISBLANK($A8),"E2:E","C2:C")&amp;MAX(INDIRECT("'"&amp;I$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1),IF(ISBLANK($A8),$B$8:$B$8,$A$8:$A$8),INDIRECT("'"&amp;I$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;I$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1)), 0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="J8" s="16">
-        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;J$1&amp;" "&amp;$A$1&amp;"'!"&amp;IF(ISBLANK($A8),"E2:E","C2:C")&amp;MAX(INDIRECT("'"&amp;J$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1),IF(ISBLANK($A8),$B$8:$B$8,$A$8:$A$8),INDIRECT("'"&amp;J$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;J$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1)), 0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="K8" s="16">
-        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;K$1&amp;" "&amp;$A$1&amp;"'!"&amp;IF(ISBLANK($A8),"E2:E","C2:C")&amp;MAX(INDIRECT("'"&amp;K$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1),IF(ISBLANK($A8),$B$8:$B$8,$A$8:$A$8),INDIRECT("'"&amp;K$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;K$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1)), 0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="L8" s="16">
-        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;L$1&amp;" "&amp;$A$1&amp;"'!"&amp;IF(ISBLANK($A8),"E2:E","C2:C")&amp;MAX(INDIRECT("'"&amp;L$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1),IF(ISBLANK($A8),$B$8:$B$8,$A$8:$A$8),INDIRECT("'"&amp;L$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;L$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1)), 0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="M8" s="16">
-        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;M$1&amp;" "&amp;$A$1&amp;"'!"&amp;IF(ISBLANK($A8),"E2:E","C2:C")&amp;MAX(INDIRECT("'"&amp;M$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1),IF(ISBLANK($A8),$B$8:$B$8,$A$8:$A$8),INDIRECT("'"&amp;M$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;M$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1)), 0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="N8" s="16">
-        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;N$1&amp;" "&amp;$A$1&amp;"'!"&amp;IF(ISBLANK($A8),"E2:E","C2:C")&amp;MAX(INDIRECT("'"&amp;N$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1),IF(ISBLANK($A8),$B$8:$B$8,$A$8:$A$8),INDIRECT("'"&amp;N$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;N$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1)), 0)</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
       <c r="O8" s="15"/>

</xml_diff>

<commit_message>
fix #16 #15 #14
</commit_message>
<xml_diff>
--- a/Budget-Book-Template.xlsx
+++ b/Budget-Book-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pfrom\Documents\GitHub\bank-account-statement-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D02BE0-B535-4113-BBC9-A3362372E9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AFE738-1BEF-409E-904B-94C97A3EFB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -30,28 +30,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1046,26 +1024,26 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="12" max="16" width="10.44140625" customWidth="1"/>
-    <col min="17" max="17" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="10.44140625" customWidth="1"/>
-    <col min="24" max="24" width="11.88671875" customWidth="1"/>
-    <col min="25" max="25" width="10.44140625" customWidth="1"/>
-    <col min="26" max="26" width="17.109375" customWidth="1"/>
+    <col min="12" max="16" width="10.42578125" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="10.42578125" customWidth="1"/>
+    <col min="24" max="24" width="11.85546875" customWidth="1"/>
+    <col min="25" max="25" width="10.42578125" customWidth="1"/>
+    <col min="26" max="26" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10">
         <v>2023</v>
       </c>
@@ -1113,57 +1091,57 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3" cm="1">
-        <f t="array" aca="1" ref="C2" ca="1">IFERROR(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="3" cm="1">
-        <f t="array" aca="1" ref="D2" ca="1">IFERROR(INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="3" cm="1">
-        <f t="array" aca="1" ref="E2" ca="1">IFERROR(INDIRECT("'"&amp;E$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;E$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="3" cm="1">
-        <f t="array" aca="1" ref="F2" ca="1">IFERROR(INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="3" cm="1">
-        <f t="array" aca="1" ref="G2" ca="1">IFERROR(INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="3" cm="1">
-        <f t="array" aca="1" ref="H2" ca="1">IFERROR(INDIRECT("'"&amp;H$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;H$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="3" cm="1">
-        <f t="array" aca="1" ref="I2" ca="1">IFERROR(INDIRECT("'"&amp;I$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;I$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="3" cm="1">
-        <f t="array" aca="1" ref="J2" ca="1">IFERROR(INDIRECT("'"&amp;J$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;J$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="3" cm="1">
-        <f t="array" aca="1" ref="K2" ca="1">IFERROR(INDIRECT("'"&amp;K$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;K$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="L2" s="3" cm="1">
-        <f t="array" aca="1" ref="L2" ca="1">IFERROR(INDIRECT("'"&amp;L$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;L$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="M2" s="3" cm="1">
-        <f t="array" aca="1" ref="M2" ca="1">IFERROR(INDIRECT("'"&amp;M$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;M$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="N2" s="3" cm="1">
-        <f t="array" aca="1" ref="N2" ca="1">IFERROR(INDIRECT("'"&amp;N$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F"&amp;MAX(INDIRECT("'"&amp;N$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))), 0)</f>
+      <c r="C2" s="3">
+        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!C:C"),$A2,INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!F:F")), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <f t="shared" ref="D2:N2" ca="1" si="0">IFERROR(SUMIF(INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!C:C"),$A2,INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!F:F")), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K2" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N2" s="3">
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="O2" s="3"/>
@@ -1173,28 +1151,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:E3" ca="1" si="0">IFERROR(SUMIF(INDIRECT("'"&amp;C1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1),"&gt;0",INDIRECT("'"&amp;C1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1)), 0)</f>
+        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;C1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))),"&gt;0",INDIRECT("'"&amp;C1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A")))), 0)</f>
         <v>0</v>
       </c>
       <c r="D3">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="D3:N3" ca="1" si="1">IFERROR(SUMIF(INDIRECT("'"&amp;D1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))),"&gt;0",INDIRECT("'"&amp;D1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A")))), 0)</f>
         <v>0</v>
       </c>
       <c r="E3">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="F3">
-        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;F1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1),"&gt;0",INDIRECT("'"&amp;F1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1)), 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:N3" ca="1" si="1">IFERROR(SUMIF(INDIRECT("'"&amp;G1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1),"&gt;0",INDIRECT("'"&amp;G1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1)), 0)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="H3">
@@ -1234,16 +1212,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:E4" ca="1" si="2">IFERROR(SUMIF(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1),"&lt;0",INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1)), 0)</f>
+        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))),"&lt;0",INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A")))), 0)</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ref="D4:N4" ca="1" si="2">IFERROR(SUMIF(INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))),"&lt;0",INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;D$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A")))), 0)</f>
         <v>0</v>
       </c>
       <c r="E4">
@@ -1251,39 +1229,39 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <f ca="1">IFERROR(SUMIF(INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1),"&lt;0",INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;F$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1)), 0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:N4" ca="1" si="3">IFERROR(SUMIF(INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1),"&lt;0",INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;G$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))-1)), 0)</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="J4">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="P4" s="6">
@@ -1295,56 +1273,56 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:N5" ca="1" si="4">SUM(C3:C4)</f>
+        <f t="shared" ref="C5:N5" ca="1" si="3">SUM(C3:C4)</f>
         <v>0</v>
       </c>
       <c r="D5">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="E5">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="F5">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="G5">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="H5">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="I5">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="J5">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="K5">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="L5">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="M5">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="N5">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="P5" s="6">
@@ -1356,12 +1334,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="14.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="4"/>
     </row>
-    <row r="7" spans="1:17" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>18</v>
       </c>
@@ -1382,57 +1360,57 @@
       <c r="P7" s="6"/>
       <c r="Q7" s="4"/>
     </row>
-    <row r="8" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="16">
-        <f t="shared" ref="C8:N8" ca="1" si="5">IFERROR(SUMIF(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;IF(ISBLANK($A8),"E2:E","C2:C")&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1),IF(ISBLANK($A8),$B$8:$B$8,$A$8:$A$8),INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1)), 0)</f>
+        <f t="shared" ref="C8:N8" ca="1" si="4">IFERROR(SUMIF(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;IF(ISBLANK($A8),"E2:E","C2:C")&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1),IF(ISBLANK($A8),$B$8:$B$8,$A$8:$A$8),INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"F2:F"&amp;MAX(INDIRECT("'"&amp;C$1&amp;" "&amp;$A$1&amp;"'!"&amp;"A:A"))+1)), 0)</f>
         <v>0</v>
       </c>
       <c r="D8" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="E8" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="F8" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="G8" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="H8" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="I8" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="J8" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="K8" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="L8" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="M8" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="N8" s="16">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="4"/>
         <v>0</v>
       </c>
       <c r="O8" s="15"/>
@@ -1445,14 +1423,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -1468,7 +1446,7 @@
       <c r="N12" s="17"/>
       <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -1484,7 +1462,7 @@
       <c r="N13" s="17"/>
       <c r="O13" s="9"/>
     </row>
-    <row r="14" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -1500,10 +1478,10 @@
       <c r="N14" s="17"/>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -1518,7 +1496,7 @@
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
     </row>
   </sheetData>

</xml_diff>